<commit_message>
Add specific ion marker for POS mode and TAG mode Bug fix: O- and P- linked residues no longer plotted and used for scoring table. DDA top # in the figure is correct now.
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/PL_specific_ion_cfg.xlsx
+++ b/ConfigurationFiles/PL_specific_ion_cfg.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="78">
   <si>
     <t>PC</t>
   </si>
@@ -175,6 +175,84 @@
   </si>
   <si>
     <t>PS:-87</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>H3O4P</t>
+  </si>
+  <si>
+    <t>[M+H]+</t>
+  </si>
+  <si>
+    <t>[M+NH4]+</t>
+  </si>
+  <si>
+    <t>C5H14NO4P</t>
+  </si>
+  <si>
+    <t>PC:183</t>
+  </si>
+  <si>
+    <t>PC:184</t>
+  </si>
+  <si>
+    <t>PA HG</t>
+  </si>
+  <si>
+    <t>PC HG</t>
+  </si>
+  <si>
+    <t>PC HG [M+H]+</t>
+  </si>
+  <si>
+    <t>C3H9N</t>
+  </si>
+  <si>
+    <t>(CH3)3N</t>
+  </si>
+  <si>
+    <t>C2H9NO4P+</t>
+  </si>
+  <si>
+    <t>C5H15NO4P+</t>
+  </si>
+  <si>
+    <t>PE:142</t>
+  </si>
+  <si>
+    <t>PE HG [M+H]+</t>
+  </si>
+  <si>
+    <t>C2H5N</t>
+  </si>
+  <si>
+    <t>PE HG part</t>
+  </si>
+  <si>
+    <t>C3H9O6P</t>
+  </si>
+  <si>
+    <t>PG HG</t>
+  </si>
+  <si>
+    <t>PG:-172</t>
+  </si>
+  <si>
+    <t>PE:-43</t>
+  </si>
+  <si>
+    <t>PC:-59</t>
+  </si>
+  <si>
+    <t>PA:-98</t>
+  </si>
+  <si>
+    <t>PS:186</t>
+  </si>
+  <si>
+    <t>C3H9NO6P+</t>
   </si>
 </sst>
 </file>
@@ -532,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,71 +648,48 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1">
-        <v>168.04580000000001</v>
+        <v>97.976898000000006</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="G2" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1">
-        <v>224.06878699999999</v>
+        <v>97.976898000000006</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="G3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1">
-        <v>242.079352</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -642,210 +697,693 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1">
-        <v>60.021129999999999</v>
+        <v>168.04580000000001</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1">
+        <v>224.06878699999999</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="1">
-        <v>140.01127199999999</v>
+        <v>242.079352</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1">
-        <v>196.037487</v>
+        <v>60.021129999999999</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>59.073498999999998</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1">
-        <v>171.005853</v>
+        <v>59.073498999999998</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="F10" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="G10" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1">
-        <v>152.99528799999999</v>
+        <v>183.066047</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="G11" t="s">
-        <v>33</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1">
+        <v>183.066047</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1">
-        <v>241.01133300000001</v>
+        <v>184.07387199999999</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="G13" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="1">
-        <v>162.05282399999999</v>
+        <v>184.07387199999999</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="F14" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="G14" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="1">
-        <v>184.001102</v>
+        <v>140.01127199999999</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
         <v>23</v>
       </c>
       <c r="F16" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G16" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="1">
-        <v>87.032028999999994</v>
+        <v>196.037487</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E17" t="s">
         <v>23</v>
       </c>
       <c r="F17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1">
+        <v>142.02692200000001</v>
+      </c>
+      <c r="D18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1">
+        <v>142.02692200000001</v>
+      </c>
+      <c r="D19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1">
+        <v>43.042198999999997</v>
+      </c>
+      <c r="D20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" t="s">
+        <v>73</v>
+      </c>
+      <c r="G20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1">
+        <v>43.042198999999997</v>
+      </c>
+      <c r="D21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="1">
+        <v>171.005853</v>
+      </c>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="1">
+        <v>152.99528799999999</v>
+      </c>
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="1">
+        <v>172.013678</v>
+      </c>
+      <c r="D25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" t="s">
+        <v>72</v>
+      </c>
+      <c r="G25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="1">
+        <v>172.013678</v>
+      </c>
+      <c r="D26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F26" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="1">
+        <v>241.01133300000001</v>
+      </c>
+      <c r="D29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" t="s">
+        <v>48</v>
+      </c>
+      <c r="G29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="1">
+        <v>162.05282399999999</v>
+      </c>
+      <c r="D30" t="s">
+        <v>36</v>
+      </c>
+      <c r="E30" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" t="s">
+        <v>49</v>
+      </c>
+      <c r="G30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="1">
+        <v>162.05282399999999</v>
+      </c>
+      <c r="D31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" t="s">
+        <v>49</v>
+      </c>
+      <c r="G31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="1">
+        <v>162.05282399999999</v>
+      </c>
+      <c r="D32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" t="s">
+        <v>49</v>
+      </c>
+      <c r="G32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="1">
+        <v>184.001102</v>
+      </c>
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" t="s">
+        <v>23</v>
+      </c>
+      <c r="F34" t="s">
+        <v>50</v>
+      </c>
+      <c r="G34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="1">
+        <v>87.032028999999994</v>
+      </c>
+      <c r="D35" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" t="s">
         <v>51</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G35" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="1">
+        <v>87.032028999999994</v>
+      </c>
+      <c r="D36" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" t="s">
+        <v>54</v>
+      </c>
+      <c r="F36" t="s">
+        <v>51</v>
+      </c>
+      <c r="G36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="1">
+        <v>87.032028999999994</v>
+      </c>
+      <c r="D37" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" t="s">
+        <v>55</v>
+      </c>
+      <c r="F37" t="s">
+        <v>51</v>
+      </c>
+      <c r="G37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="1">
+        <v>186.016752</v>
+      </c>
+      <c r="D38" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" t="s">
+        <v>54</v>
+      </c>
+      <c r="F38" t="s">
+        <v>76</v>
+      </c>
+      <c r="G38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="1">
+        <v>186.016752</v>
+      </c>
+      <c r="D39" t="s">
+        <v>77</v>
+      </c>
+      <c r="E39" t="s">
+        <v>55</v>
+      </c>
+      <c r="F39" t="s">
+        <v>76</v>
+      </c>
+      <c r="G39" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
move lipidhunter core to lib. refactor HunterCore to SpectraHunter. Add Mass shift for diff segments for Static GPF mode Bug fix: Thermo mode fix. Unspecific peak marker  update
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/PL_specific_ion_cfg.xlsx
+++ b/ConfigurationFiles/PL_specific_ion_cfg.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="81">
   <si>
     <t>PC</t>
   </si>
@@ -253,6 +253,15 @@
   </si>
   <si>
     <t>C3H9NO6P+</t>
+  </si>
+  <si>
+    <t>POS</t>
+  </si>
+  <si>
+    <t>NEG</t>
+  </si>
+  <si>
+    <t>CHARGE_MODE</t>
   </si>
 </sst>
 </file>
@@ -610,20 +619,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
-    <col min="4" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="68" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="7" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="68" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -637,16 +648,19 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>39</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -660,16 +674,19 @@
         <v>53</v>
       </c>
       <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
         <v>54</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>75</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -683,16 +700,19 @@
         <v>53</v>
       </c>
       <c r="E3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" t="s">
         <v>55</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>75</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -706,16 +726,19 @@
         <v>17</v>
       </c>
       <c r="E5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" t="s">
         <v>2</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>40</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -729,16 +752,19 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" t="s">
         <v>2</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>41</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -752,16 +778,19 @@
         <v>19</v>
       </c>
       <c r="E7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" t="s">
         <v>2</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>42</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -775,16 +804,19 @@
         <v>6</v>
       </c>
       <c r="E8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" t="s">
         <v>2</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>43</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -798,16 +830,19 @@
         <v>62</v>
       </c>
       <c r="E9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" t="s">
         <v>54</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>74</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -821,16 +856,19 @@
         <v>62</v>
       </c>
       <c r="E10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" t="s">
         <v>55</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>74</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -844,16 +882,19 @@
         <v>56</v>
       </c>
       <c r="E11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" t="s">
         <v>54</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>57</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -867,16 +908,19 @@
         <v>56</v>
       </c>
       <c r="E12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" t="s">
         <v>55</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>57</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -890,16 +934,19 @@
         <v>65</v>
       </c>
       <c r="E13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" t="s">
         <v>54</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>58</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -913,16 +960,19 @@
         <v>65</v>
       </c>
       <c r="E14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" t="s">
         <v>55</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>58</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -936,16 +986,19 @@
         <v>16</v>
       </c>
       <c r="E16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" t="s">
         <v>23</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>44</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -959,16 +1012,19 @@
         <v>18</v>
       </c>
       <c r="E17" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" t="s">
         <v>23</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>45</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -982,16 +1038,19 @@
         <v>64</v>
       </c>
       <c r="E18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" t="s">
         <v>54</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>66</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -1005,16 +1064,19 @@
         <v>64</v>
       </c>
       <c r="E19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" t="s">
         <v>55</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>66</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1028,16 +1090,19 @@
         <v>68</v>
       </c>
       <c r="E20" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" t="s">
         <v>54</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>73</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1051,16 +1116,19 @@
         <v>68</v>
       </c>
       <c r="E21" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" t="s">
         <v>55</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>73</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1074,16 +1142,19 @@
         <v>29</v>
       </c>
       <c r="E23" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" t="s">
         <v>23</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>46</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1097,16 +1168,19 @@
         <v>30</v>
       </c>
       <c r="E24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" t="s">
         <v>23</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>47</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1120,16 +1194,19 @@
         <v>70</v>
       </c>
       <c r="E25" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" t="s">
         <v>54</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>72</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1143,16 +1220,19 @@
         <v>70</v>
       </c>
       <c r="E26" t="s">
+        <v>78</v>
+      </c>
+      <c r="F26" t="s">
         <v>55</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>72</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1166,16 +1246,19 @@
         <v>35</v>
       </c>
       <c r="E29" t="s">
+        <v>79</v>
+      </c>
+      <c r="F29" t="s">
         <v>23</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>48</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1189,16 +1272,19 @@
         <v>36</v>
       </c>
       <c r="E30" t="s">
+        <v>79</v>
+      </c>
+      <c r="F30" t="s">
         <v>23</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>49</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1212,16 +1298,19 @@
         <v>36</v>
       </c>
       <c r="E31" t="s">
+        <v>78</v>
+      </c>
+      <c r="F31" t="s">
         <v>54</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>49</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1235,16 +1324,19 @@
         <v>36</v>
       </c>
       <c r="E32" t="s">
+        <v>78</v>
+      </c>
+      <c r="F32" t="s">
         <v>55</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>49</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>24</v>
       </c>
@@ -1258,16 +1350,19 @@
         <v>31</v>
       </c>
       <c r="E34" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" t="s">
         <v>23</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>50</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>24</v>
       </c>
@@ -1281,16 +1376,19 @@
         <v>25</v>
       </c>
       <c r="E35" t="s">
+        <v>79</v>
+      </c>
+      <c r="F35" t="s">
         <v>23</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>51</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>24</v>
       </c>
@@ -1304,16 +1402,19 @@
         <v>25</v>
       </c>
       <c r="E36" t="s">
+        <v>78</v>
+      </c>
+      <c r="F36" t="s">
         <v>54</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>51</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>24</v>
       </c>
@@ -1327,16 +1428,19 @@
         <v>25</v>
       </c>
       <c r="E37" t="s">
+        <v>78</v>
+      </c>
+      <c r="F37" t="s">
         <v>55</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>51</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -1350,16 +1454,19 @@
         <v>77</v>
       </c>
       <c r="E38" t="s">
+        <v>78</v>
+      </c>
+      <c r="F38" t="s">
         <v>54</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>76</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>24</v>
       </c>
@@ -1373,12 +1480,15 @@
         <v>77</v>
       </c>
       <c r="E39" t="s">
+        <v>78</v>
+      </c>
+      <c r="F39" t="s">
         <v>55</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>76</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Canopy IDE support. Bug fix: fix ppm in certain condition. Now Lyso PL has whitelist check in PL mode.
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/PL_specific_ion_cfg.xlsx
+++ b/ConfigurationFiles/PL_specific_ion_cfg.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="85">
   <si>
     <t>PC</t>
   </si>
@@ -262,6 +262,18 @@
   </si>
   <si>
     <t>CHARGE_MODE</t>
+  </si>
+  <si>
+    <t>PE HG</t>
+  </si>
+  <si>
+    <t>PE:-141</t>
+  </si>
+  <si>
+    <t>C2H8NO4P</t>
+  </si>
+  <si>
+    <t>PC:-183</t>
   </si>
 </sst>
 </file>
@@ -619,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,10 +686,10 @@
         <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
         <v>75</v>
@@ -703,7 +715,7 @@
         <v>78</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
         <v>75</v>
@@ -712,30 +724,30 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1">
-        <v>168.04580000000001</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" t="s">
-        <v>1</v>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1">
+        <v>97.976898000000006</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -746,10 +758,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="1">
-        <v>224.06878699999999</v>
+        <v>168.04580000000001</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
         <v>79</v>
@@ -758,10 +770,10 @@
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -772,10 +784,10 @@
         <v>7</v>
       </c>
       <c r="C7" s="1">
-        <v>242.079352</v>
+        <v>224.06878699999999</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
         <v>79</v>
@@ -784,10 +796,10 @@
         <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -795,13 +807,13 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1">
-        <v>60.021129999999999</v>
+        <v>242.079352</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
         <v>79</v>
@@ -810,10 +822,10 @@
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -824,22 +836,22 @@
         <v>8</v>
       </c>
       <c r="C9" s="1">
-        <v>59.073498999999998</v>
+        <v>60.021129999999999</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="H9" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -850,22 +862,22 @@
         <v>8</v>
       </c>
       <c r="C10" s="1">
-        <v>59.073498999999998</v>
+        <v>183.066047</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="G10" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="H10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -876,10 +888,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="1">
-        <v>183.066047</v>
+        <v>59.073498999999998</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
         <v>78</v>
@@ -888,10 +900,10 @@
         <v>54</v>
       </c>
       <c r="G11" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="H11" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -902,10 +914,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="1">
-        <v>183.066047</v>
+        <v>59.073498999999998</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
         <v>78</v>
@@ -914,10 +926,10 @@
         <v>55</v>
       </c>
       <c r="G12" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="H12" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -925,13 +937,13 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C13" s="1">
-        <v>184.07387199999999</v>
+        <v>183.066047</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E13" t="s">
         <v>78</v>
@@ -940,10 +952,10 @@
         <v>54</v>
       </c>
       <c r="G13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -951,13 +963,13 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C14" s="1">
-        <v>184.07387199999999</v>
+        <v>183.066047</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E14" t="s">
         <v>78</v>
@@ -966,62 +978,62 @@
         <v>55</v>
       </c>
       <c r="G14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1">
+        <v>184.07387199999999</v>
+      </c>
+      <c r="D15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" t="s">
         <v>58</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="1">
-        <v>140.01127199999999</v>
+        <v>184.07387199999999</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="E16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F16" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="G16" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="H16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="1">
-        <v>196.037487</v>
-      </c>
-      <c r="D17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" t="s">
-        <v>79</v>
-      </c>
-      <c r="F17" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" t="s">
-        <v>45</v>
-      </c>
-      <c r="H17" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1032,22 +1044,22 @@
         <v>7</v>
       </c>
       <c r="C18" s="1">
-        <v>142.02692200000001</v>
+        <v>140.01127199999999</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F18" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="G18" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="H18" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1058,22 +1070,22 @@
         <v>7</v>
       </c>
       <c r="C19" s="1">
-        <v>142.02692200000001</v>
+        <v>196.037487</v>
       </c>
       <c r="D19" t="s">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F19" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="G19" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="H19" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1084,22 +1096,22 @@
         <v>8</v>
       </c>
       <c r="C20" s="1">
-        <v>43.042198999999997</v>
+        <v>141.01909699999999</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F20" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="G20" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="H20" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1116,10 +1128,10 @@
         <v>68</v>
       </c>
       <c r="E21" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F21" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="G21" t="s">
         <v>73</v>
@@ -1128,122 +1140,174 @@
         <v>69</v>
       </c>
     </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1">
+        <v>142.02692200000001</v>
+      </c>
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="1">
-        <v>171.005853</v>
+        <v>142.02692200000001</v>
       </c>
       <c r="D23" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="E23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F23" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="G23" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="H23" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C24" s="1">
-        <v>152.99528799999999</v>
+        <v>43.042198999999997</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="E24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F24" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="G24" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="H24" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="1">
+        <v>43.042198999999997</v>
+      </c>
+      <c r="D25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" t="s">
+        <v>73</v>
+      </c>
+      <c r="H25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>28</v>
       </c>
-      <c r="B25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="1">
-        <v>172.013678</v>
-      </c>
-      <c r="D25" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" t="s">
-        <v>78</v>
-      </c>
-      <c r="F25" t="s">
-        <v>54</v>
-      </c>
-      <c r="G25" t="s">
-        <v>72</v>
-      </c>
-      <c r="H25" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="1">
+        <v>171.005853</v>
+      </c>
+      <c r="D27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" t="s">
+        <v>46</v>
+      </c>
+      <c r="H27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>28</v>
       </c>
-      <c r="B26" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="1">
-        <v>172.013678</v>
-      </c>
-      <c r="D26" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" t="s">
-        <v>78</v>
-      </c>
-      <c r="F26" t="s">
-        <v>55</v>
-      </c>
-      <c r="G26" t="s">
-        <v>72</v>
-      </c>
-      <c r="H26" t="s">
-        <v>71</v>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1">
+        <v>152.99528799999999</v>
+      </c>
+      <c r="D28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H28" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C29" s="1">
-        <v>241.01133300000001</v>
+        <v>172.013678</v>
       </c>
       <c r="D29" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="E29" t="s">
         <v>79</v>
@@ -1252,102 +1316,102 @@
         <v>23</v>
       </c>
       <c r="G29" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="H29" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
       </c>
       <c r="C30" s="1">
-        <v>162.05282399999999</v>
+        <v>172.013678</v>
       </c>
       <c r="D30" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="E30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F30" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="G30" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="H30" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="1">
+        <v>172.013678</v>
+      </c>
+      <c r="D31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" t="s">
+        <v>78</v>
+      </c>
+      <c r="F31" t="s">
+        <v>55</v>
+      </c>
+      <c r="G31" t="s">
+        <v>72</v>
+      </c>
+      <c r="H31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>34</v>
       </c>
-      <c r="B31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="1">
-        <v>162.05282399999999</v>
-      </c>
-      <c r="D31" t="s">
-        <v>36</v>
-      </c>
-      <c r="E31" t="s">
-        <v>78</v>
-      </c>
-      <c r="F31" t="s">
-        <v>54</v>
-      </c>
-      <c r="G31" t="s">
-        <v>49</v>
-      </c>
-      <c r="H31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="1">
-        <v>162.05282399999999</v>
-      </c>
-      <c r="D32" t="s">
-        <v>36</v>
-      </c>
-      <c r="E32" t="s">
-        <v>78</v>
-      </c>
-      <c r="F32" t="s">
-        <v>55</v>
-      </c>
-      <c r="G32" t="s">
-        <v>49</v>
-      </c>
-      <c r="H32" t="s">
-        <v>37</v>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="1">
+        <v>241.01133300000001</v>
+      </c>
+      <c r="D33" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" t="s">
+        <v>79</v>
+      </c>
+      <c r="F33" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" t="s">
+        <v>48</v>
+      </c>
+      <c r="H33" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C34" s="1">
-        <v>184.001102</v>
+        <v>162.05282399999999</v>
       </c>
       <c r="D34" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E34" t="s">
         <v>79</v>
@@ -1356,88 +1420,62 @@
         <v>23</v>
       </c>
       <c r="G34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H34" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="1">
-        <v>87.032028999999994</v>
+        <v>162.05282399999999</v>
       </c>
       <c r="D35" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F35" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="G35" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H35" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>8</v>
       </c>
       <c r="C36" s="1">
-        <v>87.032028999999994</v>
+        <v>162.05282399999999</v>
       </c>
       <c r="D36" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E36" t="s">
         <v>78</v>
       </c>
       <c r="F36" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G36" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H36" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>24</v>
-      </c>
-      <c r="B37" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="1">
-        <v>87.032028999999994</v>
-      </c>
-      <c r="D37" t="s">
-        <v>25</v>
-      </c>
-      <c r="E37" t="s">
-        <v>78</v>
-      </c>
-      <c r="F37" t="s">
-        <v>55</v>
-      </c>
-      <c r="G37" t="s">
-        <v>51</v>
-      </c>
-      <c r="H37" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1448,19 +1486,19 @@
         <v>7</v>
       </c>
       <c r="C38" s="1">
-        <v>186.016752</v>
+        <v>184.001102</v>
       </c>
       <c r="D38" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="E38" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F38" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="G38" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="H38" t="s">
         <v>26</v>
@@ -1471,24 +1509,128 @@
         <v>24</v>
       </c>
       <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="1">
+        <v>87.032028999999994</v>
+      </c>
+      <c r="D39" t="s">
+        <v>25</v>
+      </c>
+      <c r="E39" t="s">
+        <v>79</v>
+      </c>
+      <c r="F39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" t="s">
+        <v>51</v>
+      </c>
+      <c r="H39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="1">
+        <v>87.032028999999994</v>
+      </c>
+      <c r="D40" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" t="s">
+        <v>78</v>
+      </c>
+      <c r="F40" t="s">
+        <v>54</v>
+      </c>
+      <c r="G40" t="s">
+        <v>51</v>
+      </c>
+      <c r="H40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="1">
+        <v>87.032028999999994</v>
+      </c>
+      <c r="D41" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" t="s">
+        <v>78</v>
+      </c>
+      <c r="F41" t="s">
+        <v>55</v>
+      </c>
+      <c r="G41" t="s">
+        <v>51</v>
+      </c>
+      <c r="H41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C42" s="1">
         <v>186.016752</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D42" t="s">
         <v>77</v>
       </c>
-      <c r="E39" t="s">
-        <v>78</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="E42" t="s">
+        <v>78</v>
+      </c>
+      <c r="F42" t="s">
+        <v>54</v>
+      </c>
+      <c r="G42" t="s">
+        <v>76</v>
+      </c>
+      <c r="H42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="1">
+        <v>186.016752</v>
+      </c>
+      <c r="D43" t="s">
+        <v>77</v>
+      </c>
+      <c r="E43" t="s">
+        <v>78</v>
+      </c>
+      <c r="F43" t="s">
         <v>55</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G43" t="s">
         <v>76</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H43" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
hot fix [M+OAc]- mode for PC lipids
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/PL_specific_ion_cfg.xlsx
+++ b/ConfigurationFiles/PL_specific_ion_cfg.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="74">
   <si>
     <t>PC</t>
   </si>
@@ -229,6 +229,18 @@
   </si>
   <si>
     <t>-(serine-H2O)</t>
+  </si>
+  <si>
+    <t>[M+OAc]-</t>
+  </si>
+  <si>
+    <t>PC:-74</t>
+  </si>
+  <si>
+    <t>-CH3COOCH3</t>
+  </si>
+  <si>
+    <t>C3H6O2</t>
   </si>
 </sst>
 </file>
@@ -594,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,122 +803,148 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3">
+        <v>168.04580000000001</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="3">
-        <v>140.01127199999999</v>
+        <v>224.06878699999999</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="3">
-        <v>196.037487</v>
+        <v>242.079352</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="3">
-        <v>141.01909699999999</v>
+        <v>74.036779999999993</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="3">
-        <v>43.042198999999997</v>
+        <v>183.066047</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="3">
-        <v>171.005853</v>
+        <v>140.01127199999999</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>48</v>
@@ -915,24 +953,24 @@
         <v>17</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="3">
-        <v>152.99528799999999</v>
+        <v>196.037487</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>48</v>
@@ -941,24 +979,24 @@
         <v>17</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="3">
-        <v>172.013678</v>
+        <v>141.01909699999999</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>48</v>
@@ -967,50 +1005,50 @@
         <v>17</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="3">
-        <v>241.01133300000001</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="3">
+        <v>43.042198999999997</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>66</v>
+      <c r="G18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" s="3">
-        <v>162.05282399999999</v>
+        <v>171.005853</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>48</v>
@@ -1019,24 +1057,50 @@
         <v>17</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>67</v>
+        <v>34</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="3">
+        <v>152.99528799999999</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C22" s="3">
-        <v>184.001102</v>
+        <v>172.013678</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>48</v>
@@ -1045,35 +1109,113 @@
         <v>17</v>
       </c>
       <c r="G22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="3">
+        <v>241.01133300000001</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="3">
+        <v>162.05282399999999</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="3">
+        <v>184.001102</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H27" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B28" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C28" s="3">
         <v>87.032028999999994</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" s="5" t="s">
+      <c r="E28" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H28" s="4" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TG Score bug Fix.
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/PL_specific_ion_cfg.xlsx
+++ b/ConfigurationFiles/PL_specific_ion_cfg.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="89">
   <si>
     <t>PC</t>
   </si>
@@ -241,6 +241,51 @@
   </si>
   <si>
     <t>C3H6O2</t>
+  </si>
+  <si>
+    <t>[M+H]+</t>
+  </si>
+  <si>
+    <t>POS</t>
+  </si>
+  <si>
+    <t>NH3</t>
+  </si>
+  <si>
+    <t>TG</t>
+  </si>
+  <si>
+    <t>PC:184</t>
+  </si>
+  <si>
+    <t>PC Head Group ion in positive mode</t>
+  </si>
+  <si>
+    <t>[M+NH4]+</t>
+  </si>
+  <si>
+    <t>PE:142</t>
+  </si>
+  <si>
+    <t>PE Head Group in positive mode</t>
+  </si>
+  <si>
+    <t>C2H9O4NP-</t>
+  </si>
+  <si>
+    <t>C5H15NO4P-</t>
+  </si>
+  <si>
+    <t>C3H9NO6P-</t>
+  </si>
+  <si>
+    <t>PS:186</t>
+  </si>
+  <si>
+    <t>PS Head Group [M+H]+</t>
+  </si>
+  <si>
+    <t>TG ammonium loss</t>
   </si>
 </sst>
 </file>
@@ -279,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -291,6 +336,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -606,22 +654,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="7" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="7" width="13.5546875" customWidth="1"/>
     <col min="8" max="8" width="68" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -647,7 +695,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>40</v>
       </c>
@@ -673,7 +721,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -699,7 +747,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -725,7 +773,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
@@ -751,7 +799,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>0</v>
       </c>
@@ -777,7 +825,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
@@ -803,7 +851,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
@@ -829,7 +877,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>0</v>
       </c>
@@ -855,7 +903,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>0</v>
       </c>
@@ -881,7 +929,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>0</v>
       </c>
@@ -907,7 +955,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>0</v>
       </c>
@@ -933,33 +981,42 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="3">
-        <v>140.01127199999999</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>184.06</v>
+      </c>
+      <c r="D14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="3"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -967,10 +1024,10 @@
         <v>3</v>
       </c>
       <c r="C16" s="3">
-        <v>196.037487</v>
+        <v>140.01127199999999</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>48</v>
@@ -979,24 +1036,24 @@
         <v>17</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17" s="3">
-        <v>141.01909699999999</v>
+        <v>196.037487</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>48</v>
@@ -1005,13 +1062,13 @@
         <v>17</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>11</v>
       </c>
@@ -1019,10 +1076,10 @@
         <v>4</v>
       </c>
       <c r="C18" s="3">
-        <v>43.042198999999997</v>
+        <v>141.01909699999999</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>48</v>
@@ -1031,76 +1088,76 @@
         <v>17</v>
       </c>
       <c r="G18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="3">
+        <v>43.042198999999997</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H19" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="3">
-        <v>171.005853</v>
+        <v>142</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="3">
-        <v>152.99528799999999</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22" s="3">
-        <v>172.013678</v>
+        <v>171.005853</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>48</v>
@@ -1109,24 +1166,50 @@
         <v>17</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="3">
+        <v>152.99528799999999</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C24" s="3">
-        <v>241.01133300000001</v>
+        <v>172.013678</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>48</v>
@@ -1135,50 +1218,50 @@
         <v>17</v>
       </c>
       <c r="G24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="3">
+        <v>241.01133300000001</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C27" s="3">
         <v>162.05282399999999</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D27" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="3">
-        <v>184.001102</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>48</v>
@@ -1187,36 +1270,118 @@
         <v>17</v>
       </c>
       <c r="G27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="3">
+        <v>184.001102</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H29" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C30" s="3">
         <v>87.032028999999994</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D30" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F28" s="5" t="s">
+      <c r="E30" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H30" s="4" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="1">
+        <v>186</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="3"/>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="5">
+        <v>17.026548999999999</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>